<commit_message>
commit changes on pr and buttons
</commit_message>
<xml_diff>
--- a/export_po.xlsx
+++ b/export_po.xlsx
@@ -19,31 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Supplier:</t>
   </si>
   <si>
-    <t>Cover and Pages Corporation</t>
+    <t>Alprops Management  Inc. ( Montevista Hot Spring and Conference Resort)</t>
   </si>
   <si>
     <t>PO No.</t>
   </si>
   <si>
-    <t>2021-07-00141</t>
+    <t>2022-03-0005</t>
   </si>
   <si>
     <t>Address:</t>
   </si>
   <si>
-    <t xml:space="preserve">2763 Silang Street, Sta. Ana, Manila
- </t>
+    <t>Barangay Pansol Calamba Laguna</t>
   </si>
   <si>
     <t>DATE:</t>
   </si>
   <si>
-    <t>July 23, 2021</t>
+    <t>April 08, 2022</t>
   </si>
   <si>
     <t>Tel No.:</t>
@@ -53,9 +52,6 @@
   </si>
   <si>
     <t>Fax No.:</t>
-  </si>
-  <si>
-    <t>Small Value Procurement</t>
   </si>
   <si>
     <r>
@@ -117,23 +113,40 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>S2529</t>
+    <t>S3607</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>Specialty Paper, A4
+TEST7</t>
+  </si>
+  <si>
+    <t>S3634</t>
   </si>
   <si>
     <t>piece</t>
   </si>
   <si>
-    <t>Training Kit
-Training Manual and ECO BAG (KATYA with Design and LOGO)* Size: 210 mm x 148.5 mm  (A5)* Stock: Cover Foldcote #15* Inside: Book # 70* Color: Full* Finish: Glueing/Gathering* Process: Offset</t>
-  </si>
-  <si>
-    <t>315,368.00</t>
+    <t>Flasher
+TEST7</t>
+  </si>
+  <si>
+    <t>S3642</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>Parking Fee
+TEST7</t>
   </si>
   <si>
     <t>page 1 of 1</t>
   </si>
   <si>
-    <t>(Total Amount in Words)   Three Hundred Ten Five Thousand Three Hundred Sixty Eight pesos only</t>
+    <t>(Total Amount in Words)    pesos only</t>
   </si>
   <si>
     <t xml:space="preserve">                   In case of failure to make full delivery within time specified above, a penalty of one-tenth (1/10) of one percent for every day of delay shall be imposed.</t>
@@ -1135,15 +1148,13 @@
       <c r="B10" s="47"/>
       <c r="C10" s="6"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="48" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="48"/>
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
@@ -1154,17 +1165,17 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
       <c r="E13" s="51"/>
       <c r="F13" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="70" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="70" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1183,71 +1194,95 @@
       <c r="D15" s="51"/>
       <c r="E15" s="51"/>
       <c r="F15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" customHeight="1" ht="15.75">
       <c r="A16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="52" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>20</v>
       </c>
       <c r="D16" s="52"/>
       <c r="E16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="13" t="s">
+    </row>
+    <row r="17" spans="1:8" customHeight="1" ht="30">
+      <c r="A17" s="28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" customHeight="1" ht="63">
-      <c r="A17" s="28" t="s">
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="30" t="s">
         <v>25</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>26</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="4">
-        <v>1264</v>
+        <v>1</v>
       </c>
       <c r="F17" s="15">
-        <v>249.5</v>
-      </c>
-      <c r="G17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" customHeight="1" ht="30">
+      <c r="A18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" customHeight="1" ht="15">
-      <c r="A18" s="15"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="30"/>
+      <c r="C18" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="D18" s="31"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="15"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="30"/>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="15">
+        <v>400</v>
+      </c>
+      <c r="G18" s="15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" customHeight="1" ht="30">
+      <c r="A19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>31</v>
+      </c>
       <c r="D19" s="31"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="15">
+        <v>150</v>
+      </c>
+      <c r="G19" s="15">
+        <v>450</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="15"/>
@@ -1496,7 +1531,7 @@
       <c r="A47" s="16"/>
       <c r="B47" s="5"/>
       <c r="C47" s="36" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D47" s="37"/>
       <c r="E47" s="6"/>
@@ -1505,15 +1540,15 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="38" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B48" s="38"/>
       <c r="C48" s="39"/>
       <c r="D48" s="39"/>
       <c r="E48" s="38"/>
       <c r="F48" s="38"/>
-      <c r="G48" s="40" t="s">
-        <v>27</v>
+      <c r="G48" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1531,7 +1566,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="43" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -1552,51 +1587,51 @@
     <row r="53" spans="1:8" customHeight="1" ht="7.15"/>
     <row r="54" spans="1:8">
       <c r="E54" s="44" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:8">
       <c r="E56" s="29" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C58" s="6"/>
       <c r="E58" s="45" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F58" s="45"/>
       <c r="G58" s="45"/>
     </row>
     <row r="59" spans="1:8">
       <c r="E59" s="46" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F59" s="46"/>
       <c r="G59" s="46"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="55" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B60" s="56"/>
       <c r="C60" s="56"/>
       <c r="D60" s="57"/>
       <c r="E60" s="34" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="34"/>
@@ -1613,7 +1648,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
@@ -1624,7 +1659,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="58" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="58"/>
@@ -1774,7 +1809,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
@@ -1785,14 +1820,14 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="50" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
       <c r="E13" s="51"/>
       <c r="F13" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -1803,7 +1838,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="51"/>
       <c r="F14" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -1814,29 +1849,29 @@
       <c r="D15" s="51"/>
       <c r="E15" s="51"/>
       <c r="F15" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:8" customHeight="1" ht="15.75">
       <c r="A16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="52" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>20</v>
       </c>
       <c r="D16" s="52"/>
       <c r="E16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1933,7 +1968,7 @@
       <c r="A27" s="15"/>
       <c r="B27" s="3"/>
       <c r="C27" s="30" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D27" s="31"/>
       <c r="E27" s="4"/>
@@ -1944,7 +1979,7 @@
       <c r="A28" s="15"/>
       <c r="B28" s="3"/>
       <c r="C28" s="32" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="4"/>
@@ -1955,7 +1990,7 @@
       <c r="A29" s="15"/>
       <c r="B29" s="3"/>
       <c r="C29" s="32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="4"/>
@@ -1966,7 +2001,7 @@
       <c r="A30" s="15"/>
       <c r="B30" s="3"/>
       <c r="C30" s="32" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="4"/>
@@ -2121,7 +2156,7 @@
       <c r="A47" s="16"/>
       <c r="B47" s="5"/>
       <c r="C47" s="60" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D47" s="61"/>
       <c r="E47" s="6"/>
@@ -2130,7 +2165,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="62" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B48" s="62"/>
       <c r="C48" s="63"/>
@@ -2154,7 +2189,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="43" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -2175,39 +2210,39 @@
     <row r="53" spans="1:8" customHeight="1" ht="7.15"/>
     <row r="54" spans="1:8">
       <c r="E54" s="44" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:8">
       <c r="E56" s="29" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C58" s="6"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="34" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B60" s="34"/>
       <c r="C60" s="34"/>
       <c r="D60" s="34"/>
       <c r="E60" s="34" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="34"/>

</xml_diff>